<commit_message>
round 2 ties and app fixes
</commit_message>
<xml_diff>
--- a/data/DreamLeague25-26.xlsx
+++ b/data/DreamLeague25-26.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/462a734c48854128/Desktop/Dream League/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="8_{7D36DF2E-EA78-4237-9818-EA41DFB80887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD7FE276-ECB6-4F2C-9EE2-5E39A3DFFEB8}"/>
+  <xr:revisionPtr revIDLastSave="531" documentId="8_{7D36DF2E-EA78-4237-9818-EA41DFB80887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5F67F5-37A2-414A-8C71-0E7AB33D3481}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="464">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1413,6 +1413,24 @@
   </si>
   <si>
     <t>BRADFORD</t>
+  </si>
+  <si>
+    <t>NEWLL'S OLD TIKI TAKA</t>
+  </si>
+  <si>
+    <t>WOODHALL SPA WHITES</t>
+  </si>
+  <si>
+    <t>BETTER TOGETHER</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE ULSTERMEN</t>
+  </si>
+  <si>
+    <t>OWEN BAILEY</t>
+  </si>
+  <si>
+    <t>ZAN VIPOTNIK</t>
   </si>
 </sst>
 </file>
@@ -3331,7 +3349,7 @@
   <dimension ref="A1:IX404"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G318" sqref="G318"/>
+      <selection activeCell="K5" sqref="K5:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3469,7 +3487,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="83"/>
       <c r="H5" s="84"/>
@@ -3485,15 +3503,15 @@
       </c>
       <c r="M5" s="18">
         <f t="shared" ref="M5:M17" si="0">N5-O5</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N5" s="19">
         <f>SUM(F8:F25)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O5" s="20">
         <f>SUM(F5:F7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S5" s="102"/>
       <c r="T5" s="101"/>
@@ -3520,15 +3538,15 @@
       </c>
       <c r="M6" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N6" s="26">
         <f>SUM(F35:F52)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="O6" s="27">
         <f>SUM(F32:F34)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S6" s="102"/>
       <c r="T6" s="101"/>
@@ -3555,15 +3573,15 @@
       </c>
       <c r="M7" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N7" s="26">
         <f>SUM(F62:F79)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O7" s="27">
         <f>SUM(F59:F61)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S7" s="102"/>
       <c r="T7" s="101"/>
@@ -3599,15 +3617,15 @@
       </c>
       <c r="M8" s="25">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="26">
         <f>SUM(F89:F106)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O8" s="27">
         <f>SUM(F86:F88)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3641,7 +3659,7 @@
       </c>
       <c r="M9" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N9" s="73">
         <f>SUM(F116:F133)</f>
@@ -3649,7 +3667,7 @@
       </c>
       <c r="O9" s="74">
         <f>SUM(F113:F115)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3673,15 +3691,15 @@
       </c>
       <c r="M10" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N10" s="26">
         <f>SUM(F143:F160)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O10" s="27">
         <f>SUM(F140:F142)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R10" s="117"/>
       <c r="S10" s="117"/>
@@ -3704,7 +3722,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="87"/>
       <c r="H11" s="84"/>
@@ -3720,15 +3738,15 @@
       </c>
       <c r="M11" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N11" s="26">
         <f>SUM(F170:F187)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="O11" s="27">
         <f>SUM(F167:F169)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S11" s="102"/>
       <c r="T11" s="101"/>
@@ -3736,23 +3754,27 @@
     </row>
     <row r="12" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="79"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="108" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="109">
         <v>1</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="110">
         <v>0</v>
       </c>
-      <c r="G12" s="87"/>
-      <c r="H12" s="84"/>
+      <c r="G12" s="87" t="s">
+        <v>292</v>
+      </c>
+      <c r="H12" s="84">
+        <v>45932</v>
+      </c>
       <c r="I12" s="99"/>
       <c r="J12" s="82"/>
       <c r="K12" s="71" t="str">
@@ -3765,15 +3787,15 @@
       </c>
       <c r="M12" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N12" s="73">
         <f>SUM(F197:F214)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O12" s="74">
         <f>SUM(F194:F196)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3782,18 +3804,20 @@
         <v>16</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>188</v>
+        <v>462</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="29">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>291</v>
       </c>
       <c r="F13" s="30">
-        <v>1</v>
-      </c>
-      <c r="G13" s="87"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="87">
+        <v>45932</v>
+      </c>
       <c r="H13" s="84"/>
       <c r="I13" s="99"/>
       <c r="J13" s="82"/>
@@ -3807,15 +3831,15 @@
       </c>
       <c r="M13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N13" s="73">
         <f>SUM(F224:F241)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O13" s="74">
         <f>SUM(F221:F223)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="R13" s="117"/>
       <c r="S13" s="117"/>
@@ -3825,11 +3849,21 @@
     </row>
     <row r="14" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
+      <c r="B14" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="30">
+        <v>2</v>
+      </c>
       <c r="G14" s="87"/>
       <c r="H14" s="84"/>
       <c r="I14" s="99"/>
@@ -3844,15 +3878,15 @@
       </c>
       <c r="M14" s="25">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="N14" s="73">
         <f>SUM(F251:F268)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O14" s="74">
         <f>SUM(F248:F250)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="S14" s="102"/>
       <c r="T14" s="101"/>
@@ -3879,15 +3913,15 @@
       </c>
       <c r="M15" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N15" s="26">
         <f>SUM(F277:F295)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O15" s="27">
         <f>SUM(F275:F276)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3911,15 +3945,15 @@
       </c>
       <c r="M16" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N16" s="26">
         <f>SUM(F305:F322)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="O16" s="27">
         <f>SUM(F302:F304)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3957,15 +3991,15 @@
       </c>
       <c r="M17" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N17" s="26">
         <f>SUM(F332:F349)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O17" s="27">
         <f>SUM(F329:F331)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R17" s="117"/>
       <c r="S17" s="117"/>
@@ -4006,15 +4040,15 @@
       </c>
       <c r="M18" s="25">
         <f>N18-O18</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N18" s="26">
         <f>SUM(F359:F376)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O18" s="27">
         <f>SUM(F356:F358)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S18" s="102"/>
       <c r="T18" s="101"/>
@@ -4085,25 +4119,27 @@
     </row>
     <row r="21" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="79"/>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="108" t="s">
         <v>298</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="108" t="s">
         <v>299</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="109" t="s">
         <v>291</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="110">
         <v>0</v>
       </c>
       <c r="G21" s="87">
         <v>45883</v>
       </c>
-      <c r="H21" s="84"/>
+      <c r="H21" s="84">
+        <v>45932</v>
+      </c>
       <c r="I21" s="99"/>
       <c r="J21" s="76"/>
       <c r="K21" s="1"/>
@@ -4121,18 +4157,20 @@
         <v>17</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>190</v>
+        <v>463</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="29">
-        <v>8</v>
+        <v>136</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>291</v>
       </c>
       <c r="F22" s="30">
-        <v>3</v>
-      </c>
-      <c r="G22" s="87"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="87">
+        <v>45932</v>
+      </c>
       <c r="H22" s="84"/>
       <c r="I22" s="89"/>
       <c r="J22" s="76"/>
@@ -4144,27 +4182,23 @@
     </row>
     <row r="23" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="79"/>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="108" t="s">
-        <v>191</v>
-      </c>
-      <c r="D23" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="109">
-        <v>1</v>
-      </c>
-      <c r="F23" s="110">
-        <v>1</v>
-      </c>
-      <c r="G23" s="87" t="s">
-        <v>292</v>
-      </c>
-      <c r="H23" s="84">
-        <v>45911</v>
-      </c>
+      <c r="C23" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="29">
+        <v>8</v>
+      </c>
+      <c r="F23" s="30">
+        <v>3</v>
+      </c>
+      <c r="G23" s="87"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="89"/>
       <c r="J23" s="76"/>
       <c r="K23" s="1"/>
@@ -4175,25 +4209,27 @@
     </row>
     <row r="24" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="79"/>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>435</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="F24" s="30">
-        <v>0</v>
-      </c>
-      <c r="G24" s="87">
+      <c r="C24" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="108" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="109">
+        <v>1</v>
+      </c>
+      <c r="F24" s="110">
+        <v>1</v>
+      </c>
+      <c r="G24" s="87" t="s">
+        <v>292</v>
+      </c>
+      <c r="H24" s="84">
         <v>45911</v>
       </c>
-      <c r="H24" s="84"/>
       <c r="I24" s="89"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -4209,12 +4245,24 @@
     </row>
     <row r="25" spans="1:22" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="79"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="87"/>
+      <c r="B25" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="F25" s="30">
+        <v>1</v>
+      </c>
+      <c r="G25" s="87">
+        <v>45911</v>
+      </c>
       <c r="H25" s="84"/>
       <c r="I25" s="89"/>
       <c r="J25" s="76"/>
@@ -4238,7 +4286,7 @@
       </c>
       <c r="F26" s="36">
         <f>SUM(F8:F25)-SUM(F5:F7)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G26" s="80"/>
       <c r="H26" s="92"/>
@@ -4367,13 +4415,11 @@
         <v>1</v>
       </c>
       <c r="F32" s="15">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G32" s="80"/>
       <c r="H32" s="94"/>
-      <c r="I32" s="95">
-        <v>-3</v>
-      </c>
+      <c r="I32" s="95"/>
       <c r="J32" s="76"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -4457,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="91"/>
       <c r="H36" s="91"/>
@@ -4501,13 +4547,11 @@
         <v>32</v>
       </c>
       <c r="F38" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" s="83"/>
       <c r="H38" s="91"/>
-      <c r="I38" s="93">
-        <v>1</v>
-      </c>
+      <c r="I38" s="93"/>
       <c r="J38" s="76"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -4535,7 +4579,7 @@
         <v>12</v>
       </c>
       <c r="F39" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39" s="87"/>
       <c r="H39" s="91"/>
@@ -4562,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G40" s="87"/>
       <c r="H40" s="91"/>
@@ -4671,7 +4715,7 @@
         <v>291</v>
       </c>
       <c r="F45" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="87">
         <v>45876</v>
@@ -4887,7 +4931,7 @@
       </c>
       <c r="F53" s="36">
         <f>SUM(F35:F52)-SUM(F32:F34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G53" s="80"/>
       <c r="H53" s="92"/>
@@ -5011,7 +5055,7 @@
         <v>4</v>
       </c>
       <c r="F59" s="15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G59" s="80"/>
       <c r="H59" s="92"/>
@@ -5143,7 +5187,7 @@
         <v>30</v>
       </c>
       <c r="F65" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" s="83"/>
       <c r="H65" s="90"/>
@@ -5170,13 +5214,11 @@
         <v>5</v>
       </c>
       <c r="F66" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G66" s="83"/>
       <c r="H66" s="91"/>
-      <c r="I66" s="90">
-        <v>1</v>
-      </c>
+      <c r="I66" s="90"/>
       <c r="J66" s="76"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -5230,15 +5272,13 @@
         <v>291</v>
       </c>
       <c r="F68" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" s="91">
         <v>45904</v>
       </c>
       <c r="H68" s="91"/>
-      <c r="I68" s="90">
-        <v>1</v>
-      </c>
+      <c r="I68" s="90"/>
       <c r="J68" s="76"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -5526,7 +5566,7 @@
       </c>
       <c r="F80" s="36">
         <f>SUM(F62:F79)-SUM(F59:F61)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G80" s="80"/>
       <c r="H80" s="92"/>
@@ -5650,13 +5690,11 @@
         <v>8</v>
       </c>
       <c r="F86" s="15">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G86" s="80"/>
       <c r="H86" s="94"/>
-      <c r="I86" s="93">
-        <v>-3</v>
-      </c>
+      <c r="I86" s="93"/>
       <c r="J86" s="76"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
@@ -5871,7 +5909,7 @@
         <v>19</v>
       </c>
       <c r="F95" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="91"/>
       <c r="H95" s="91"/>
@@ -5932,7 +5970,7 @@
         <v>25</v>
       </c>
       <c r="F98" s="30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G98" s="87"/>
       <c r="H98" s="91"/>
@@ -6011,13 +6049,13 @@
         <v>453</v>
       </c>
       <c r="D101" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E101" s="29" t="s">
         <v>291</v>
       </c>
       <c r="F101" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G101" s="87">
         <v>45918</v>
@@ -6110,9 +6148,7 @@
         <v>45911</v>
       </c>
       <c r="H104" s="91"/>
-      <c r="I104" s="90">
-        <v>1</v>
-      </c>
+      <c r="I104" s="90"/>
       <c r="J104" s="76"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
@@ -6165,7 +6201,7 @@
       </c>
       <c r="F107" s="36">
         <f>SUM(F89:F106)-SUM(F86:F88)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G107" s="80"/>
       <c r="H107" s="92"/>
@@ -6289,13 +6325,11 @@
         <v>1</v>
       </c>
       <c r="F113" s="15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G113" s="80"/>
       <c r="H113" s="94"/>
-      <c r="I113" s="90">
-        <v>-1</v>
-      </c>
+      <c r="I113" s="90"/>
       <c r="J113" s="76"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
@@ -6427,9 +6461,7 @@
       </c>
       <c r="G119" s="87"/>
       <c r="H119" s="91"/>
-      <c r="I119" s="90">
-        <v>1</v>
-      </c>
+      <c r="I119" s="90"/>
       <c r="J119" s="76"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
@@ -6708,9 +6740,7 @@
       </c>
       <c r="G130" s="87"/>
       <c r="H130" s="91"/>
-      <c r="I130" s="90">
-        <v>1</v>
-      </c>
+      <c r="I130" s="90"/>
       <c r="J130" s="76"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
@@ -6737,9 +6767,7 @@
       </c>
       <c r="G131" s="87"/>
       <c r="H131" s="91"/>
-      <c r="I131" s="90">
-        <v>1</v>
-      </c>
+      <c r="I131" s="90"/>
       <c r="J131" s="76"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
@@ -6792,7 +6820,7 @@
       </c>
       <c r="F134" s="36">
         <f>SUM(F116:F133)-SUM(F113:F115)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G134" s="80"/>
       <c r="H134" s="92"/>
@@ -6945,7 +6973,7 @@
         <v>438</v>
       </c>
       <c r="F141" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G141" s="86">
         <v>45911</v>
@@ -7062,13 +7090,11 @@
         <v>42</v>
       </c>
       <c r="F146" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G146" s="87"/>
       <c r="H146" s="90"/>
-      <c r="I146" s="90">
-        <v>1</v>
-      </c>
+      <c r="I146" s="90"/>
       <c r="J146" s="76"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
@@ -7091,12 +7117,10 @@
         <v>1</v>
       </c>
       <c r="F147" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H147" s="103"/>
-      <c r="I147" s="90">
-        <v>1</v>
-      </c>
+      <c r="I147" s="90"/>
       <c r="J147" s="76"/>
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
@@ -7224,7 +7248,7 @@
         <v>18</v>
       </c>
       <c r="F153" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G153" s="83"/>
       <c r="H153" s="91"/>
@@ -7338,7 +7362,7 @@
         <v>4</v>
       </c>
       <c r="F157" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G157" s="87"/>
       <c r="H157" s="91"/>
@@ -7412,7 +7436,7 @@
       </c>
       <c r="F161" s="36">
         <f>SUM(F143:F160)-SUM(F140:F142)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G161" s="80"/>
       <c r="H161" s="92"/>
@@ -7536,7 +7560,7 @@
         <v>1</v>
       </c>
       <c r="F167" s="15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G167" s="80"/>
       <c r="H167" s="94"/>
@@ -7668,13 +7692,11 @@
         <v>3</v>
       </c>
       <c r="F173" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G173" s="83"/>
       <c r="H173" s="91"/>
-      <c r="I173" s="90">
-        <v>1</v>
-      </c>
+      <c r="I173" s="90"/>
       <c r="J173" s="76"/>
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
@@ -7757,7 +7779,7 @@
         <v>1</v>
       </c>
       <c r="F176" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G176" s="91"/>
       <c r="H176" s="91"/>
@@ -7818,7 +7840,7 @@
         <v>56</v>
       </c>
       <c r="F179" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G179" s="87"/>
       <c r="H179" s="91"/>
@@ -8033,7 +8055,7 @@
       </c>
       <c r="F188" s="36">
         <f>SUM(F170:F187)-SUM(F167:F169)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G188" s="87"/>
       <c r="H188" s="91"/>
@@ -8157,7 +8179,7 @@
         <v>1</v>
       </c>
       <c r="F194" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G194" s="80"/>
       <c r="H194" s="94"/>
@@ -8425,9 +8447,7 @@
       </c>
       <c r="G206" s="87"/>
       <c r="H206" s="90"/>
-      <c r="I206" s="90">
-        <v>1</v>
-      </c>
+      <c r="I206" s="90"/>
       <c r="J206" s="76"/>
       <c r="K206" s="1"/>
       <c r="L206" s="1"/>
@@ -8454,9 +8474,7 @@
       </c>
       <c r="G207" s="83"/>
       <c r="H207" s="90"/>
-      <c r="I207" s="90">
-        <v>1</v>
-      </c>
+      <c r="I207" s="90"/>
       <c r="J207" s="76"/>
       <c r="K207" s="1"/>
       <c r="L207" s="1"/>
@@ -8506,7 +8524,7 @@
         <v>1</v>
       </c>
       <c r="F209" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G209" s="87"/>
       <c r="H209" s="91"/>
@@ -8624,7 +8642,7 @@
       </c>
       <c r="F215" s="36">
         <f>SUM(F197:F214)-SUM(F194:F196)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G215" s="80"/>
       <c r="H215" s="92"/>
@@ -8777,15 +8795,13 @@
         <v>291</v>
       </c>
       <c r="F222" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G222" s="94">
         <v>45890</v>
       </c>
       <c r="H222" s="92"/>
-      <c r="I222" s="89">
-        <v>-1</v>
-      </c>
+      <c r="I222" s="89"/>
       <c r="J222" s="76"/>
       <c r="K222" s="1"/>
       <c r="L222" s="1"/>
@@ -8852,7 +8868,7 @@
         <v>5</v>
       </c>
       <c r="F225" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G225" s="87"/>
       <c r="H225" s="91"/>
@@ -8927,7 +8943,7 @@
         <v>291</v>
       </c>
       <c r="F228" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G228" s="87">
         <v>45918</v>
@@ -9064,9 +9080,7 @@
       </c>
       <c r="G233" s="87"/>
       <c r="H233" s="91"/>
-      <c r="I233" s="89">
-        <v>1</v>
-      </c>
+      <c r="I233" s="89"/>
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
       <c r="L233" s="1"/>
@@ -9089,7 +9103,7 @@
         <v>20</v>
       </c>
       <c r="F234" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G234" s="87"/>
       <c r="H234" s="91"/>
@@ -9120,9 +9134,7 @@
       </c>
       <c r="G235" s="83"/>
       <c r="H235" s="91"/>
-      <c r="I235" s="89">
-        <v>1</v>
-      </c>
+      <c r="I235" s="89"/>
       <c r="J235" s="76"/>
       <c r="K235" s="1"/>
       <c r="L235" s="1"/>
@@ -9203,7 +9215,7 @@
         <v>291</v>
       </c>
       <c r="F238" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G238" s="87">
         <v>45911</v>
@@ -9279,7 +9291,7 @@
       </c>
       <c r="F242" s="36">
         <f>SUM(F224:F241)-SUM(F221:F223)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G242" s="80"/>
       <c r="H242" s="92"/>
@@ -9403,9 +9415,7 @@
       <c r="H248" s="94">
         <v>45918</v>
       </c>
-      <c r="I248" s="90">
-        <v>-5</v>
-      </c>
+      <c r="I248" s="90"/>
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
       <c r="L248" s="1"/>
@@ -9426,7 +9436,7 @@
         <v>291</v>
       </c>
       <c r="F249" s="21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G249" s="86">
         <v>45918</v>
@@ -9718,7 +9728,7 @@
         <v>18</v>
       </c>
       <c r="F261" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G261" s="87"/>
       <c r="H261" s="91"/>
@@ -9906,7 +9916,7 @@
       </c>
       <c r="F269" s="36">
         <f>SUM(F251:F268)-SUM(F248:F250)</f>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="G269" s="80"/>
       <c r="H269" s="92"/>
@@ -10030,7 +10040,7 @@
         <v>1</v>
       </c>
       <c r="F275" s="15">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G275" s="80"/>
       <c r="H275" s="94"/>
@@ -10310,7 +10320,7 @@
         <v>12</v>
       </c>
       <c r="F287" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G287" s="87"/>
       <c r="H287" s="91"/>
@@ -10341,9 +10351,7 @@
       </c>
       <c r="G288" s="87"/>
       <c r="H288" s="91"/>
-      <c r="I288" s="90">
-        <v>1</v>
-      </c>
+      <c r="I288" s="90"/>
       <c r="J288" s="1"/>
       <c r="K288" s="1"/>
       <c r="L288" s="1"/>
@@ -10420,7 +10428,7 @@
         <v>1</v>
       </c>
       <c r="F291" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G291" s="87"/>
       <c r="H291" s="91"/>
@@ -10511,7 +10519,7 @@
       </c>
       <c r="F296" s="36">
         <f>SUM(F278:F295)-SUM(F275:F276)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G296" s="91"/>
       <c r="H296" s="91"/>
@@ -10664,7 +10672,7 @@
         <v>291</v>
       </c>
       <c r="F303" s="21">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G303" s="87">
         <v>45890</v>
@@ -10781,7 +10789,7 @@
         <v>4</v>
       </c>
       <c r="F308" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G308" s="87"/>
       <c r="H308" s="91"/>
@@ -10929,13 +10937,11 @@
         <v>54</v>
       </c>
       <c r="F314" s="30">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G314" s="87"/>
       <c r="H314" s="91"/>
-      <c r="I314" s="90">
-        <v>2</v>
-      </c>
+      <c r="I314" s="90"/>
       <c r="J314" s="1"/>
       <c r="K314" s="1"/>
       <c r="L314" s="1"/>
@@ -10962,9 +10968,7 @@
       </c>
       <c r="G315" s="87"/>
       <c r="H315" s="91"/>
-      <c r="I315" s="90">
-        <v>1</v>
-      </c>
+      <c r="I315" s="90"/>
       <c r="J315" s="1"/>
       <c r="K315" s="1"/>
       <c r="L315" s="1"/>
@@ -10987,13 +10991,11 @@
         <v>1</v>
       </c>
       <c r="F316" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G316" s="87"/>
       <c r="H316" s="91"/>
-      <c r="I316" s="90">
-        <v>1</v>
-      </c>
+      <c r="I316" s="90"/>
       <c r="J316" s="1"/>
       <c r="K316" s="1"/>
       <c r="L316" s="1"/>
@@ -11107,7 +11109,7 @@
         <v>291</v>
       </c>
       <c r="F320" s="30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G320" s="87">
         <v>45890</v>
@@ -11166,7 +11168,7 @@
       </c>
       <c r="F323" s="36">
         <f>SUM(F305:F322)-SUM(F302:F304)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G323" s="80"/>
       <c r="H323" s="92"/>
@@ -11290,7 +11292,7 @@
         <v>1</v>
       </c>
       <c r="F329" s="15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G329" s="83"/>
       <c r="H329" s="87"/>
@@ -11552,9 +11554,7 @@
       </c>
       <c r="G341" s="83"/>
       <c r="H341" s="91"/>
-      <c r="I341" s="90">
-        <v>1</v>
-      </c>
+      <c r="I341" s="90"/>
       <c r="J341" s="1"/>
       <c r="N341" s="1"/>
       <c r="O341" s="1"/>
@@ -11574,7 +11574,7 @@
         <v>1</v>
       </c>
       <c r="F342" s="30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G342" s="87"/>
       <c r="H342" s="91"/>
@@ -11598,7 +11598,7 @@
         <v>1</v>
       </c>
       <c r="F343" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G343" s="87"/>
       <c r="H343" s="91"/>
@@ -11622,13 +11622,11 @@
         <v>1</v>
       </c>
       <c r="F344" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G344" s="83"/>
       <c r="H344" s="91"/>
-      <c r="I344" s="90">
-        <v>3</v>
-      </c>
+      <c r="I344" s="90"/>
       <c r="J344" s="1"/>
       <c r="N344" s="1"/>
       <c r="O344" s="1"/>
@@ -11724,7 +11722,7 @@
       </c>
       <c r="F350" s="36">
         <f>SUM(F332:F349)-SUM(F329:F331)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G350" s="83"/>
       <c r="H350" s="90"/>
@@ -11806,13 +11804,11 @@
         <v>5</v>
       </c>
       <c r="F356" s="15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G356" s="1"/>
       <c r="H356" s="104"/>
-      <c r="I356" s="1">
-        <v>-1</v>
-      </c>
+      <c r="I356" s="1"/>
       <c r="J356" s="1"/>
     </row>
     <row r="357" spans="2:10" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11872,7 +11868,7 @@
         <v>1</v>
       </c>
       <c r="F360" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G360" s="1"/>
       <c r="H360" s="1"/>
@@ -11929,9 +11925,7 @@
       </c>
       <c r="G363" s="1"/>
       <c r="H363" s="104"/>
-      <c r="I363" s="1">
-        <v>1</v>
-      </c>
+      <c r="I363" s="1"/>
       <c r="J363" s="1"/>
     </row>
     <row r="364" spans="2:10" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -12039,7 +12033,7 @@
         <v>12</v>
       </c>
       <c r="F369" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G369" s="104"/>
       <c r="H369" s="104"/>
@@ -12060,7 +12054,7 @@
         <v>5</v>
       </c>
       <c r="F370" s="30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G370" s="104"/>
       <c r="H370" s="1"/>
@@ -12081,7 +12075,7 @@
         <v>1</v>
       </c>
       <c r="F371" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G371" s="1"/>
       <c r="H371" s="104"/>
@@ -12179,7 +12173,7 @@
       </c>
       <c r="F377" s="36">
         <f>SUM(F359:F376)-SUM(F356:F358)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G377" s="1"/>
       <c r="H377" s="1"/>
@@ -12435,7 +12429,7 @@
   <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12559,13 +12553,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="26">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G7" s="27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="41"/>
@@ -12580,22 +12574,22 @@
       <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="55" t="s">
         <v>202</v>
       </c>
       <c r="E8" s="25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="26">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G8" s="27">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H8" s="52"/>
       <c r="I8" s="41"/>
       <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="K8" s="53"/>
     </row>
     <row r="9" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
@@ -12603,19 +12597,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>207</v>
+        <v>99</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>237</v>
       </c>
       <c r="E9" s="25">
-        <v>9</v>
-      </c>
-      <c r="F9" s="56">
-        <v>19</v>
-      </c>
-      <c r="G9" s="57">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="26">
+        <v>22</v>
+      </c>
+      <c r="G9" s="27">
+        <v>15</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="41"/>
@@ -12628,19 +12622,19 @@
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>273</v>
+        <v>33</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>32</v>
       </c>
       <c r="E10" s="25">
-        <v>6</v>
-      </c>
-      <c r="F10" s="26">
-        <v>13</v>
-      </c>
-      <c r="G10" s="27">
         <v>7</v>
+      </c>
+      <c r="F10" s="56">
+        <v>18</v>
+      </c>
+      <c r="G10" s="57">
+        <v>11</v>
       </c>
       <c r="H10" s="52"/>
       <c r="I10" s="41"/>
@@ -12650,22 +12644,22 @@
     <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>32</v>
+        <v>55</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>273</v>
       </c>
       <c r="E11" s="25">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F11" s="26">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G11" s="27">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H11" s="52"/>
       <c r="I11" s="41"/>
@@ -12680,17 +12674,17 @@
       <c r="C12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="55" t="s">
         <v>248</v>
       </c>
       <c r="E12" s="25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12" s="26">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G12" s="27">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="41"/>
@@ -12703,19 +12697,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>237</v>
+        <v>52</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>207</v>
       </c>
       <c r="E13" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="26">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G13" s="27">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H13" s="52"/>
       <c r="I13" s="41"/>
@@ -12728,19 +12722,19 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>142</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="E14" s="25">
-        <v>3</v>
-      </c>
-      <c r="F14" s="56">
-        <v>9</v>
-      </c>
-      <c r="G14" s="57">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="F14" s="26">
+        <v>11</v>
+      </c>
+      <c r="G14" s="27">
+        <v>7</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="41"/>
@@ -12753,19 +12747,19 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>192</v>
       </c>
       <c r="E15" s="25">
         <v>2</v>
       </c>
-      <c r="F15" s="26">
-        <v>8</v>
-      </c>
-      <c r="G15" s="27">
-        <v>6</v>
+      <c r="F15" s="56">
+        <v>12</v>
+      </c>
+      <c r="G15" s="57">
+        <v>10</v>
       </c>
       <c r="H15" s="52"/>
       <c r="I15" s="41"/>
@@ -12778,19 +12772,19 @@
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>54</v>
+        <v>249</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>250</v>
       </c>
       <c r="E16" s="25">
-        <v>2</v>
-      </c>
-      <c r="F16" s="26">
-        <v>5</v>
-      </c>
-      <c r="G16" s="27">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F16" s="56">
+        <v>13</v>
+      </c>
+      <c r="G16" s="57">
+        <v>12</v>
       </c>
       <c r="H16" s="52"/>
       <c r="I16" s="41"/>
@@ -12803,24 +12797,24 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>192</v>
+        <v>53</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="E17" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17" s="27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" s="52"/>
       <c r="I17" s="41"/>
       <c r="J17" s="41"/>
-      <c r="K17" s="53"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
@@ -12830,17 +12824,17 @@
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="24" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="25">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="26">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G18" s="27">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H18" s="52"/>
       <c r="I18" s="41"/>
@@ -12850,22 +12844,22 @@
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
       <c r="B19" s="54">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
         <v>12</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="E19" s="25">
-        <v>-1</v>
-      </c>
-      <c r="F19" s="26">
-        <v>8</v>
-      </c>
       <c r="G19" s="27">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H19" s="52"/>
       <c r="I19" s="41"/>
@@ -12880,17 +12874,17 @@
       <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="24" t="s">
         <v>226</v>
       </c>
       <c r="E20" s="25">
-        <v>-10</v>
-      </c>
-      <c r="F20" s="56">
-        <v>4</v>
-      </c>
-      <c r="G20" s="57">
-        <v>14</v>
+        <v>-12</v>
+      </c>
+      <c r="F20" s="26">
+        <v>5</v>
+      </c>
+      <c r="G20" s="27">
+        <v>17</v>
       </c>
       <c r="H20" s="52"/>
       <c r="I20" s="41"/>
@@ -13265,7 +13259,7 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -13366,13 +13360,13 @@
       <c r="D4" s="64" t="s">
         <v>445</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="100">
         <v>-1</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="100" t="s">
         <v>450</v>
       </c>
       <c r="H4" s="38"/>
@@ -13408,13 +13402,13 @@
       <c r="D5" s="64" t="s">
         <v>443</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="100">
         <v>0</v>
       </c>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="100" t="s">
         <v>449</v>
       </c>
       <c r="H5" s="38"/>
@@ -13450,13 +13444,13 @@
       <c r="D6" s="64" t="s">
         <v>443</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="69" t="s">
         <v>422</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="100">
         <v>0</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="100" t="s">
         <v>446</v>
       </c>
       <c r="H6" s="38"/>
@@ -13492,13 +13486,13 @@
       <c r="D7" s="64" t="s">
         <v>441</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="69" t="s">
         <v>423</v>
       </c>
-      <c r="F7" s="64">
+      <c r="F7" s="100">
         <v>1</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="100" t="s">
         <v>444</v>
       </c>
       <c r="H7" s="38"/>
@@ -13525,13 +13519,13 @@
       <c r="A8" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="69" t="s">
         <v>250</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="100">
         <v>0</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="100" t="s">
         <v>446</v>
       </c>
       <c r="E8" s="68" t="s">
@@ -13567,13 +13561,13 @@
       <c r="A9" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="100">
         <v>-2</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="100" t="s">
         <v>442</v>
       </c>
       <c r="E9" s="68" t="s">
@@ -13609,13 +13603,13 @@
       <c r="A10" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="100">
         <v>1</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="100" t="s">
         <v>444</v>
       </c>
       <c r="E10" s="68" t="s">
@@ -13691,13 +13685,13 @@
       <c r="A12" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="69" t="s">
         <v>428</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="100">
         <v>-2</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="100" t="s">
         <v>442</v>
       </c>
       <c r="E12" s="68" t="s">
@@ -13740,13 +13734,13 @@
       <c r="D13" s="64" t="s">
         <v>441</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="69" t="s">
         <v>430</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="100">
         <v>1</v>
       </c>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="100" t="s">
         <v>443</v>
       </c>
       <c r="H13" s="38"/>
@@ -13828,13 +13822,21 @@
       <c r="B16" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="68" t="s">
+      <c r="C16" s="64">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>450</v>
+      </c>
+      <c r="E16" s="69" t="s">
         <v>427</v>
       </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
+      <c r="F16" s="100">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="100" t="s">
+        <v>447</v>
+      </c>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
@@ -13911,10 +13913,14 @@
       <c r="A19" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="65"/>
+      <c r="B19" s="65" t="s">
+        <v>248</v>
+      </c>
       <c r="C19" s="68"/>
       <c r="D19" s="64"/>
-      <c r="E19" s="70"/>
+      <c r="E19" s="65" t="s">
+        <v>54</v>
+      </c>
       <c r="F19" s="69"/>
       <c r="G19" s="100"/>
       <c r="H19" s="38"/>
@@ -13939,10 +13945,14 @@
       <c r="A20" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="65"/>
+      <c r="B20" s="65" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="68"/>
       <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
+      <c r="E20" s="65" t="s">
+        <v>424</v>
+      </c>
       <c r="F20" s="68"/>
       <c r="G20" s="64"/>
       <c r="H20" s="38"/>
@@ -13967,10 +13977,14 @@
       <c r="A21" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="65"/>
+      <c r="B21" s="65" t="s">
+        <v>142</v>
+      </c>
       <c r="C21" s="68"/>
       <c r="D21" s="64"/>
-      <c r="E21" s="70"/>
+      <c r="E21" s="65" t="s">
+        <v>426</v>
+      </c>
       <c r="F21" s="69"/>
       <c r="G21" s="100"/>
       <c r="H21" s="38"/>
@@ -13995,10 +14009,14 @@
       <c r="A22" s="67" t="s">
         <v>261</v>
       </c>
-      <c r="B22" s="70"/>
+      <c r="B22" s="65" t="s">
+        <v>54</v>
+      </c>
       <c r="C22" s="69"/>
       <c r="D22" s="100"/>
-      <c r="E22" s="65"/>
+      <c r="E22" s="65" t="s">
+        <v>202</v>
+      </c>
       <c r="F22" s="68"/>
       <c r="G22" s="64"/>
       <c r="H22" s="38"/>
@@ -14023,10 +14041,14 @@
       <c r="A23" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="B23" s="70"/>
+      <c r="B23" s="65" t="s">
+        <v>458</v>
+      </c>
       <c r="C23" s="69"/>
       <c r="D23" s="100"/>
-      <c r="E23" s="65"/>
+      <c r="E23" s="65" t="s">
+        <v>425</v>
+      </c>
       <c r="F23" s="68"/>
       <c r="G23" s="64"/>
       <c r="H23" s="38"/>
@@ -14051,10 +14073,14 @@
       <c r="A24" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="70"/>
+      <c r="B24" s="65" t="s">
+        <v>429</v>
+      </c>
       <c r="C24" s="69"/>
       <c r="D24" s="100"/>
-      <c r="E24" s="65"/>
+      <c r="E24" s="65" t="s">
+        <v>459</v>
+      </c>
       <c r="F24" s="68"/>
       <c r="G24" s="64"/>
       <c r="H24" s="38"/>
@@ -14079,10 +14105,14 @@
       <c r="A25" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="B25" s="70"/>
+      <c r="B25" s="65" t="s">
+        <v>207</v>
+      </c>
       <c r="C25" s="69"/>
       <c r="D25" s="100"/>
-      <c r="E25" s="65"/>
+      <c r="E25" s="65" t="s">
+        <v>460</v>
+      </c>
       <c r="F25" s="68"/>
       <c r="G25" s="64"/>
       <c r="H25" s="38"/>
@@ -14107,10 +14137,14 @@
       <c r="A26" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="B26" s="70"/>
+      <c r="B26" s="65" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="69"/>
       <c r="D26" s="100"/>
-      <c r="E26" s="65"/>
+      <c r="E26" s="65" t="s">
+        <v>461</v>
+      </c>
       <c r="F26" s="68"/>
       <c r="G26" s="64"/>
       <c r="H26" s="38"/>
@@ -15127,7 +15161,7 @@
   <dimension ref="A5:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19:J22"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -15408,7 +15442,7 @@
       </c>
       <c r="K13">
         <f>COUNTIF(Stats!D:D,'Player Count'!J13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="111"/>
       <c r="N13" t="s">
@@ -15504,7 +15538,7 @@
       </c>
       <c r="K16">
         <f>COUNTIF(Stats!D:D,'Player Count'!J16)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" s="111"/>
       <c r="N16" s="67" t="s">
@@ -15817,7 +15851,7 @@
       </c>
       <c r="G26">
         <f>COUNTIF(Stats!D:D,'Player Count'!F26)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" t="s">
         <v>368</v>
@@ -15857,7 +15891,7 @@
       </c>
       <c r="O27">
         <f>COUNTIF(Stats!D:D,'Player Count'!N27)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q27" s="111"/>
     </row>
@@ -15915,7 +15949,7 @@
       </c>
       <c r="G30" s="78">
         <f>SUM(G6:G29)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J30" s="78" t="s">
         <v>325</v>
@@ -15929,7 +15963,7 @@
       </c>
       <c r="O30" s="78">
         <f>SUM(O6:O29)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -15938,28 +15972,28 @@
       </c>
       <c r="C38" s="116">
         <f>C26/SUM(C26,G30,K30,O30)</f>
-        <v>0.4157303370786517</v>
+        <v>0.41111111111111109</v>
       </c>
       <c r="D38" s="116"/>
       <c r="E38" s="116"/>
       <c r="F38" s="116"/>
       <c r="G38" s="116">
         <f>G30/SUM(C26,G30,K30,O30)</f>
-        <v>0.24719101123595505</v>
+        <v>0.25</v>
       </c>
       <c r="H38" s="116"/>
       <c r="I38" s="116"/>
       <c r="J38" s="116"/>
       <c r="K38" s="116">
         <f>K30/SUM(C26,G30,K30,O30)</f>
-        <v>0.1797752808988764</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="L38" s="116"/>
       <c r="M38" s="116"/>
       <c r="N38" s="116"/>
       <c r="O38" s="116">
         <f>O30/SUM(C26,G30,K30,O30)</f>
-        <v>0.15730337078651685</v>
+        <v>0.16111111111111112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bfl qf squad list
</commit_message>
<xml_diff>
--- a/data/DreamLeague25-26.xlsx
+++ b/data/DreamLeague25-26.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/462a734c48854128/Desktop/Dream League/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1106" documentId="8_{7D36DF2E-EA78-4237-9818-EA41DFB80887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80082099-87FD-42E7-A982-9C2864572695}"/>
+  <xr:revisionPtr revIDLastSave="1143" documentId="8_{7D36DF2E-EA78-4237-9818-EA41DFB80887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02A3271-5B6E-41A5-917D-A552C7BA3921}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="488">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1500,6 +1500,9 @@
   </si>
   <si>
     <t>VICTOR TORP</t>
+  </si>
+  <si>
+    <t>EPHRON MASON-CLARK</t>
   </si>
 </sst>
 </file>
@@ -2224,11 +2227,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2315,6 +2318,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3422,8 +3429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IX404"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3542,11 +3549,11 @@
       <c r="O4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
     </row>
     <row r="5" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
@@ -3612,11 +3619,11 @@
       </c>
       <c r="M6" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N6" s="26">
         <f>SUM(F35:F52)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O6" s="27">
         <f>SUM(F32:F34)</f>
@@ -3765,21 +3772,21 @@
       </c>
       <c r="M10" s="25">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N10" s="26">
         <f>SUM(F143:F160)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O10" s="27">
         <f>SUM(F140:F142)</f>
         <v>20</v>
       </c>
-      <c r="R10" s="118"/>
-      <c r="S10" s="118"/>
-      <c r="T10" s="118"/>
-      <c r="U10" s="118"/>
-      <c r="V10" s="118"/>
+      <c r="R10" s="120"/>
+      <c r="S10" s="120"/>
+      <c r="T10" s="120"/>
+      <c r="U10" s="120"/>
+      <c r="V10" s="120"/>
     </row>
     <row r="11" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="79"/>
@@ -3915,11 +3922,11 @@
         <f>SUM(F221:F223)</f>
         <v>22</v>
       </c>
-      <c r="R13" s="118"/>
-      <c r="S13" s="118"/>
-      <c r="T13" s="118"/>
-      <c r="U13" s="118"/>
-      <c r="V13" s="118"/>
+      <c r="R13" s="120"/>
+      <c r="S13" s="120"/>
+      <c r="T13" s="120"/>
+      <c r="U13" s="120"/>
+      <c r="V13" s="120"/>
     </row>
     <row r="14" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
@@ -4075,11 +4082,11 @@
         <f>SUM(F329:F331)</f>
         <v>12</v>
       </c>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="118"/>
-      <c r="V17" s="118"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="120"/>
+      <c r="U17" s="120"/>
+      <c r="V17" s="120"/>
     </row>
     <row r="18" spans="1:22" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="79"/>
@@ -4185,11 +4192,11 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="118"/>
-      <c r="U20" s="118"/>
-      <c r="V20" s="118"/>
+      <c r="R20" s="120"/>
+      <c r="S20" s="120"/>
+      <c r="T20" s="120"/>
+      <c r="U20" s="120"/>
+      <c r="V20" s="120"/>
     </row>
     <row r="21" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="79"/>
@@ -4311,11 +4318,11 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="R24" s="118"/>
-      <c r="S24" s="118"/>
-      <c r="T24" s="118"/>
-      <c r="U24" s="118"/>
-      <c r="V24" s="118"/>
+      <c r="R24" s="120"/>
+      <c r="S24" s="120"/>
+      <c r="T24" s="120"/>
+      <c r="U24" s="120"/>
+      <c r="V24" s="120"/>
     </row>
     <row r="25" spans="1:22" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="79"/>
@@ -4405,11 +4412,11 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="R28" s="118"/>
-      <c r="S28" s="118"/>
-      <c r="T28" s="118"/>
-      <c r="U28" s="118"/>
-      <c r="V28" s="118"/>
+      <c r="R28" s="120"/>
+      <c r="S28" s="120"/>
+      <c r="T28" s="120"/>
+      <c r="U28" s="120"/>
+      <c r="V28" s="120"/>
     </row>
     <row r="29" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
@@ -4632,11 +4639,11 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="R38" s="118"/>
-      <c r="S38" s="118"/>
-      <c r="T38" s="118"/>
-      <c r="U38" s="118"/>
-      <c r="V38" s="118"/>
+      <c r="R38" s="120"/>
+      <c r="S38" s="120"/>
+      <c r="T38" s="120"/>
+      <c r="U38" s="120"/>
+      <c r="V38" s="120"/>
     </row>
     <row r="39" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="79"/>
@@ -4936,7 +4943,7 @@
         <v>288</v>
       </c>
       <c r="F50" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" s="91">
         <v>45904</v>
@@ -5005,7 +5012,7 @@
       </c>
       <c r="F53" s="36">
         <f>SUM(F35:F52)-SUM(F32:F34)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G53" s="80"/>
       <c r="H53" s="92"/>
@@ -6588,23 +6595,27 @@
     </row>
     <row r="121" spans="1:15" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="79"/>
-      <c r="B121" s="28" t="s">
+      <c r="B121" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="C121" s="28" t="s">
+      <c r="C121" s="107" t="s">
         <v>180</v>
       </c>
-      <c r="D121" s="28" t="s">
+      <c r="D121" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="E121" s="29">
+      <c r="E121" s="108">
         <v>1</v>
       </c>
-      <c r="F121" s="30">
+      <c r="F121" s="109">
         <v>1</v>
       </c>
-      <c r="G121" s="86"/>
-      <c r="H121" s="94"/>
+      <c r="G121" s="86" t="s">
+        <v>289</v>
+      </c>
+      <c r="H121" s="94">
+        <v>45974</v>
+      </c>
       <c r="I121" s="90"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -6615,12 +6626,24 @@
     </row>
     <row r="122" spans="1:15" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="79"/>
-      <c r="B122" s="28"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="28"/>
-      <c r="E122" s="29"/>
-      <c r="F122" s="30"/>
-      <c r="G122" s="87"/>
+      <c r="B122" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C122" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="D122" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E122" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="F122" s="30">
+        <v>0</v>
+      </c>
+      <c r="G122" s="87">
+        <v>45974</v>
+      </c>
       <c r="H122" s="91"/>
       <c r="I122" s="90"/>
       <c r="J122" s="76"/>
@@ -7455,7 +7478,7 @@
         <v>288</v>
       </c>
       <c r="F155" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G155" s="87">
         <v>45911</v>
@@ -7585,7 +7608,7 @@
       </c>
       <c r="F161" s="36">
         <f>SUM(F143:F160)-SUM(F140:F142)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G161" s="80"/>
       <c r="H161" s="92"/>
@@ -10280,23 +10303,27 @@
       <c r="N274" s="1"/>
       <c r="O274" s="1"/>
     </row>
-    <row r="275" spans="1:15" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A275" s="79"/>
-      <c r="B275" s="12" t="s">
+      <c r="B275" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="C275" s="13"/>
-      <c r="D275" s="12" t="s">
+      <c r="C275" s="112"/>
+      <c r="D275" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="E275" s="14">
+      <c r="E275" s="113">
         <v>1</v>
       </c>
-      <c r="F275" s="15">
+      <c r="F275" s="114">
         <v>27</v>
       </c>
-      <c r="G275" s="80"/>
-      <c r="H275" s="94"/>
+      <c r="G275" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="H275" s="94">
+        <v>45974</v>
+      </c>
       <c r="I275" s="92"/>
       <c r="J275" s="1"/>
       <c r="K275" s="1"/>
@@ -10307,12 +10334,22 @@
     </row>
     <row r="276" spans="1:15" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="79"/>
-      <c r="B276" s="21"/>
+      <c r="B276" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="C276" s="21"/>
-      <c r="D276" s="21"/>
-      <c r="E276" s="22"/>
-      <c r="F276" s="21"/>
-      <c r="G276" s="86"/>
+      <c r="D276" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E276" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="F276" s="21">
+        <v>0</v>
+      </c>
+      <c r="G276" s="86">
+        <v>45974</v>
+      </c>
       <c r="H276" s="92"/>
       <c r="I276" s="92"/>
       <c r="J276" s="1"/>
@@ -12771,8 +12808,8 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12886,7 +12923,7 @@
     </row>
     <row r="7" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47"/>
-      <c r="B7" s="120">
+      <c r="B7" s="119">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -12915,21 +12952,21 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="E8" s="25">
         <v>17</v>
       </c>
-      <c r="F8" s="56">
-        <v>32</v>
-      </c>
-      <c r="G8" s="57">
-        <v>15</v>
-      </c>
-      <c r="H8" s="119"/>
+      <c r="F8" s="26">
+        <v>37</v>
+      </c>
+      <c r="G8" s="27">
+        <v>20</v>
+      </c>
+      <c r="H8" s="52"/>
       <c r="I8" s="41"/>
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
@@ -12940,34 +12977,34 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="25">
+        <v>17</v>
+      </c>
+      <c r="F9" s="56">
         <v>32</v>
       </c>
-      <c r="D9" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="25">
-        <v>16</v>
-      </c>
-      <c r="F9" s="56">
-        <v>36</v>
-      </c>
       <c r="G9" s="57">
-        <v>20</v>
-      </c>
-      <c r="H9" s="119"/>
+        <v>15</v>
+      </c>
+      <c r="H9" s="118"/>
       <c r="I9" s="41"/>
       <c r="J9" s="41"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
-      <c r="B10" s="120">
+      <c r="B10" s="119">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="55" t="s">
         <v>248</v>
       </c>
       <c r="E10" s="25">
@@ -12979,10 +13016,10 @@
       <c r="G10" s="27">
         <v>21</v>
       </c>
-      <c r="H10" s="119"/>
+      <c r="H10" s="118"/>
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
@@ -13036,25 +13073,25 @@
     </row>
     <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
-      <c r="B13" s="120">
+      <c r="B13" s="119">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="24" t="s">
         <v>246</v>
       </c>
       <c r="E13" s="25">
         <v>8</v>
       </c>
-      <c r="F13" s="56">
+      <c r="F13" s="26">
         <v>20</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G13" s="27">
         <v>12</v>
       </c>
-      <c r="H13" s="119"/>
+      <c r="H13" s="118"/>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
@@ -13096,22 +13133,22 @@
         <v>191</v>
       </c>
       <c r="E15" s="25">
-        <v>4</v>
-      </c>
-      <c r="F15" s="26">
-        <v>23</v>
-      </c>
-      <c r="G15" s="27">
+        <v>5</v>
+      </c>
+      <c r="F15" s="56">
+        <v>24</v>
+      </c>
+      <c r="G15" s="57">
         <v>19</v>
       </c>
-      <c r="H15" s="52"/>
+      <c r="H15" s="118"/>
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
-      <c r="B16" s="120">
+      <c r="B16" s="119">
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -13129,7 +13166,7 @@
       <c r="G16" s="27">
         <v>20</v>
       </c>
-      <c r="H16" s="52"/>
+      <c r="H16" s="118"/>
       <c r="I16" s="41"/>
       <c r="J16" s="41"/>
       <c r="K16" s="41"/>
@@ -13154,7 +13191,7 @@
       <c r="G17" s="27">
         <v>27</v>
       </c>
-      <c r="H17" s="119"/>
+      <c r="H17" s="118"/>
       <c r="I17" s="41"/>
       <c r="J17" s="41"/>
       <c r="K17" s="41"/>
@@ -13186,25 +13223,25 @@
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
-      <c r="B19" s="120">
+      <c r="B19" s="119">
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="55" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="25">
         <v>-3</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="56">
         <v>16</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="57">
         <v>19</v>
       </c>
-      <c r="H19" s="119"/>
+      <c r="H19" s="118"/>
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
       <c r="K19" s="41"/>
@@ -13217,7 +13254,7 @@
       <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="24" t="s">
         <v>225</v>
       </c>
       <c r="E20" s="25">
@@ -13229,10 +13266,10 @@
       <c r="G20" s="27">
         <v>27</v>
       </c>
-      <c r="H20" s="119"/>
+      <c r="H20" s="52"/>
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
-      <c r="K20" s="53"/>
+      <c r="K20" s="41"/>
     </row>
     <row r="21" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
@@ -13602,7 +13639,7 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -14630,10 +14667,14 @@
       <c r="A29" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="B29" s="70"/>
+      <c r="B29" s="65" t="s">
+        <v>141</v>
+      </c>
       <c r="C29" s="69"/>
       <c r="D29" s="100"/>
-      <c r="E29" s="65"/>
+      <c r="E29" s="65" t="s">
+        <v>236</v>
+      </c>
       <c r="F29" s="68"/>
       <c r="G29" s="64"/>
       <c r="H29" s="38"/>
@@ -14654,14 +14695,18 @@
       <c r="W29" s="38"/>
       <c r="X29" s="38"/>
     </row>
-    <row r="30" spans="1:24" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="B30" s="63"/>
+      <c r="B30" s="65" t="s">
+        <v>34</v>
+      </c>
       <c r="C30" s="64"/>
       <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
+      <c r="E30" s="65" t="s">
+        <v>31</v>
+      </c>
       <c r="F30" s="66"/>
       <c r="G30" s="40"/>
       <c r="H30" s="38"/>
@@ -14682,14 +14727,18 @@
       <c r="W30" s="38"/>
       <c r="X30" s="38"/>
     </row>
-    <row r="31" spans="1:24" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="B31" s="63"/>
+      <c r="B31" s="65" t="s">
+        <v>246</v>
+      </c>
       <c r="C31" s="64"/>
       <c r="D31" s="64"/>
-      <c r="E31" s="65"/>
+      <c r="E31" s="65" t="s">
+        <v>426</v>
+      </c>
       <c r="F31" s="66"/>
       <c r="G31" s="40"/>
       <c r="H31" s="38"/>
@@ -14710,14 +14759,18 @@
       <c r="W31" s="38"/>
       <c r="X31" s="38"/>
     </row>
-    <row r="32" spans="1:24" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="67" t="s">
         <v>266</v>
       </c>
-      <c r="B32" s="63"/>
+      <c r="B32" s="65" t="s">
+        <v>201</v>
+      </c>
       <c r="C32" s="64"/>
       <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
+      <c r="E32" s="65" t="s">
+        <v>206</v>
+      </c>
       <c r="F32" s="66"/>
       <c r="G32" s="40"/>
       <c r="H32" s="38"/>
@@ -15746,7 +15799,7 @@
       </c>
       <c r="G10">
         <f>COUNTIF(Stats!D:D,'Player Count'!F10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J10" s="67" t="s">
         <v>351</v>
@@ -16265,7 +16318,7 @@
       </c>
       <c r="K26">
         <f>COUNTIF(Stats!D:D,'Player Count'!J26)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M26" s="110"/>
       <c r="N26" s="67" t="s">
@@ -16356,14 +16409,14 @@
       </c>
       <c r="G30" s="78">
         <f>SUM(G6:G29)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J30" s="78" t="s">
         <v>322</v>
       </c>
       <c r="K30" s="78">
         <f>SUM(K6:K29)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N30" s="78" t="s">
         <v>322</v>
@@ -16379,28 +16432,28 @@
       </c>
       <c r="C38" s="115">
         <f>C26/SUM(C26,G30,K30,O30)</f>
-        <v>0.39195979899497485</v>
+        <v>0.38805970149253732</v>
       </c>
       <c r="D38" s="115"/>
       <c r="E38" s="115"/>
       <c r="F38" s="115"/>
       <c r="G38" s="115">
         <f>G30/SUM(C26,G30,K30,O30)</f>
-        <v>0.271356783919598</v>
+        <v>0.27363184079601988</v>
       </c>
       <c r="H38" s="115"/>
       <c r="I38" s="115"/>
       <c r="J38" s="115"/>
       <c r="K38" s="115">
         <f>K30/SUM(C26,G30,K30,O30)</f>
-        <v>0.18592964824120603</v>
+        <v>0.1890547263681592</v>
       </c>
       <c r="L38" s="115"/>
       <c r="M38" s="115"/>
       <c r="N38" s="115"/>
       <c r="O38" s="115">
         <f>O30/SUM(C26,G30,K30,O30)</f>
-        <v>0.15075376884422109</v>
+        <v>0.14925373134328357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>